<commit_message>
Listed out manual corrections to artery_tcl
added to tmc_qc_25m.xlsx
</commit_message>
<xml_diff>
--- a/tmc_qc.xlsx
+++ b/tmc_qc.xlsx
@@ -731,9 +731,6 @@
     <t>Minor Arterial Ramp</t>
   </si>
   <si>
-    <t>change</t>
-  </si>
-  <si>
     <t>Ok</t>
   </si>
   <si>
@@ -1059,6 +1056,9 @@
   </si>
   <si>
     <t>change W to 8128</t>
+  </si>
+  <si>
+    <t>change S to 445260</t>
   </si>
 </sst>
 </file>
@@ -1392,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K731"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E229" sqref="E229:E234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1436,10 +1436,10 @@
         <v>221</v>
       </c>
       <c r="I1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J1" t="s">
         <v>337</v>
-      </c>
-      <c r="J1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1471,7 +1471,7 @@
         <v>224</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1503,7 +1503,7 @@
         <v>223</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1535,7 +1535,7 @@
         <v>225</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1567,7 +1567,7 @@
         <v>226</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1593,7 +1593,7 @@
         <v>225</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1840,7 +1840,7 @@
         <v>226</v>
       </c>
       <c r="J14" t="s">
-        <v>235</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1895,7 +1895,7 @@
         <v>225</v>
       </c>
       <c r="J16" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1927,7 +1927,7 @@
         <v>225</v>
       </c>
       <c r="J17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -2014,7 +2014,7 @@
         <v>225</v>
       </c>
       <c r="J20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -2037,7 +2037,7 @@
         <v>229</v>
       </c>
       <c r="J21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -2394,7 +2394,7 @@
         <v>225</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -2426,7 +2426,7 @@
         <v>225</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -2452,7 +2452,7 @@
         <v>224</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -2478,7 +2478,7 @@
         <v>225</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -2504,7 +2504,7 @@
         <v>224</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -2530,7 +2530,7 @@
         <v>225</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -2626,7 +2626,7 @@
         <v>226</v>
       </c>
       <c r="J41" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -2887,7 +2887,7 @@
         <v>225</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -2919,7 +2919,7 @@
         <v>225</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -2983,7 +2983,7 @@
         <v>225</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -3009,7 +3009,7 @@
         <v>223</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -3224,7 +3224,7 @@
         <v>227</v>
       </c>
       <c r="J61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -3311,7 +3311,7 @@
         <v>225</v>
       </c>
       <c r="J64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -3558,7 +3558,7 @@
         <v>229</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -3590,7 +3590,7 @@
         <v>225</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -3642,7 +3642,7 @@
         <v>223</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
@@ -3668,7 +3668,7 @@
         <v>229</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -3772,7 +3772,7 @@
         <v>225</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -4097,7 +4097,7 @@
         <v>223</v>
       </c>
       <c r="J91" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
@@ -4216,7 +4216,7 @@
         <v>225</v>
       </c>
       <c r="J95" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
@@ -4248,7 +4248,7 @@
         <v>225</v>
       </c>
       <c r="J96" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -4280,7 +4280,7 @@
         <v>229</v>
       </c>
       <c r="J97" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
@@ -4367,7 +4367,7 @@
         <v>223</v>
       </c>
       <c r="J100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -4390,7 +4390,7 @@
         <v>229</v>
       </c>
       <c r="J101" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
@@ -4517,7 +4517,7 @@
         <v>229</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
@@ -4549,7 +4549,7 @@
         <v>225</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
@@ -4581,7 +4581,7 @@
         <v>225</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
@@ -4613,7 +4613,7 @@
         <v>229</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
@@ -4639,7 +4639,7 @@
         <v>225</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -4964,7 +4964,7 @@
         <v>227</v>
       </c>
       <c r="J121" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
@@ -5051,7 +5051,7 @@
         <v>227</v>
       </c>
       <c r="J124" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
@@ -5074,7 +5074,7 @@
         <v>228</v>
       </c>
       <c r="J125" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
@@ -5614,7 +5614,7 @@
         <v>227</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
@@ -5646,7 +5646,7 @@
         <v>225</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
@@ -5672,7 +5672,7 @@
         <v>225</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
@@ -6235,7 +6235,7 @@
         <v>229</v>
       </c>
       <c r="J164" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
@@ -6377,7 +6377,7 @@
         <v>225</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
@@ -6435,7 +6435,7 @@
         <v>225</v>
       </c>
       <c r="J171" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.2">
@@ -6833,7 +6833,7 @@
         <v>225</v>
       </c>
       <c r="J184" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
@@ -6856,7 +6856,7 @@
         <v>225</v>
       </c>
       <c r="J185" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
@@ -6879,7 +6879,7 @@
         <v>228</v>
       </c>
       <c r="J186" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
@@ -6975,7 +6975,7 @@
         <v>225</v>
       </c>
       <c r="J189" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
@@ -7053,7 +7053,7 @@
         <v>225</v>
       </c>
       <c r="J192" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.2">
@@ -7140,7 +7140,7 @@
         <v>230</v>
       </c>
       <c r="J195" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.2">
@@ -7163,7 +7163,7 @@
         <v>225</v>
       </c>
       <c r="J196" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.2">
@@ -7195,7 +7195,7 @@
         <v>228</v>
       </c>
       <c r="J197" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
@@ -7314,7 +7314,7 @@
         <v>225</v>
       </c>
       <c r="J201" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.2">
@@ -7346,7 +7346,7 @@
         <v>225</v>
       </c>
       <c r="J202" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.2">
@@ -7433,7 +7433,7 @@
         <v>228</v>
       </c>
       <c r="J205" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.2">
@@ -7456,7 +7456,7 @@
         <v>225</v>
       </c>
       <c r="J206" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
@@ -8202,7 +8202,7 @@
         <v>225</v>
       </c>
       <c r="J231" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.2">
@@ -8234,7 +8234,7 @@
         <v>227</v>
       </c>
       <c r="J232" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.2">
@@ -8312,7 +8312,7 @@
         <v>225</v>
       </c>
       <c r="J235" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.2">
@@ -8344,7 +8344,7 @@
         <v>227</v>
       </c>
       <c r="J236" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
@@ -8376,7 +8376,7 @@
         <v>227</v>
       </c>
       <c r="J237" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.2">
@@ -8408,7 +8408,7 @@
         <v>225</v>
       </c>
       <c r="J238" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.2">
@@ -8628,7 +8628,7 @@
         <v>227</v>
       </c>
       <c r="J246" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.2">
@@ -8724,7 +8724,7 @@
         <v>225</v>
       </c>
       <c r="J249" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.2">
@@ -8747,7 +8747,7 @@
         <v>228</v>
       </c>
       <c r="J250" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.2">
@@ -8770,7 +8770,7 @@
         <v>225</v>
       </c>
       <c r="J251" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">
@@ -8834,7 +8834,7 @@
         <v>226</v>
       </c>
       <c r="J253" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.2">
@@ -8924,7 +8924,7 @@
         <v>226</v>
       </c>
       <c r="J256" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.2">
@@ -8988,7 +8988,7 @@
         <v>225</v>
       </c>
       <c r="J258" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.2">
@@ -9043,7 +9043,7 @@
         <v>228</v>
       </c>
       <c r="J260" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.2">
@@ -9066,7 +9066,7 @@
         <v>225</v>
       </c>
       <c r="J261" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.2">
@@ -9130,7 +9130,7 @@
         <v>223</v>
       </c>
       <c r="J263" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.2">
@@ -9220,7 +9220,7 @@
         <v>223</v>
       </c>
       <c r="J266" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.2">
@@ -9403,7 +9403,7 @@
         <v>225</v>
       </c>
       <c r="J272" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.2">
@@ -9435,7 +9435,7 @@
         <v>227</v>
       </c>
       <c r="J273" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.2">
@@ -9467,7 +9467,7 @@
         <v>227</v>
       </c>
       <c r="J274" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.2">
@@ -9499,7 +9499,7 @@
         <v>225</v>
       </c>
       <c r="J275" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.2">
@@ -9525,7 +9525,7 @@
         <v>223</v>
       </c>
       <c r="J276" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.2">
@@ -9653,7 +9653,7 @@
         <v>225</v>
       </c>
       <c r="J280" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.2">
@@ -9679,7 +9679,7 @@
         <v>223</v>
       </c>
       <c r="J281" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.2">
@@ -10004,7 +10004,7 @@
         <v>225</v>
       </c>
       <c r="J292" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.2">
@@ -10091,7 +10091,7 @@
         <v>228</v>
       </c>
       <c r="J295" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
@@ -10114,7 +10114,7 @@
         <v>225</v>
       </c>
       <c r="J296" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.2">
@@ -10146,7 +10146,7 @@
         <v>225</v>
       </c>
       <c r="J297" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.2">
@@ -10233,7 +10233,7 @@
         <v>225</v>
       </c>
       <c r="J300" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.2">
@@ -10256,7 +10256,7 @@
         <v>224</v>
       </c>
       <c r="J301" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.2">
@@ -10471,7 +10471,7 @@
         <v>223</v>
       </c>
       <c r="J308" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.2">
@@ -10561,7 +10561,7 @@
         <v>223</v>
       </c>
       <c r="J311" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.2">
@@ -10776,7 +10776,7 @@
         <v>225</v>
       </c>
       <c r="J318" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.2">
@@ -10808,7 +10808,7 @@
         <v>225</v>
       </c>
       <c r="J319" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.2">
@@ -10840,7 +10840,7 @@
         <v>225</v>
       </c>
       <c r="J320" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.2">
@@ -10866,7 +10866,7 @@
         <v>225</v>
       </c>
       <c r="J321" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.2">
@@ -10892,7 +10892,7 @@
         <v>225</v>
       </c>
       <c r="J322" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.2">
@@ -10918,7 +10918,7 @@
         <v>225</v>
       </c>
       <c r="J323" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.2">
@@ -10982,7 +10982,7 @@
         <v>232</v>
       </c>
       <c r="J325" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.2">
@@ -11124,7 +11124,7 @@
         <v>232</v>
       </c>
       <c r="J330" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.2">
@@ -11449,7 +11449,7 @@
         <v>225</v>
       </c>
       <c r="J341" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.2">
@@ -11472,7 +11472,7 @@
         <v>225</v>
       </c>
       <c r="J342" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.2">
@@ -11495,7 +11495,7 @@
         <v>229</v>
       </c>
       <c r="J343" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.2">
@@ -11527,7 +11527,7 @@
         <v>225</v>
       </c>
       <c r="J344" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="345" spans="1:10" x14ac:dyDescent="0.2">
@@ -11559,7 +11559,7 @@
         <v>225</v>
       </c>
       <c r="J345" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="346" spans="1:10" x14ac:dyDescent="0.2">
@@ -11591,7 +11591,7 @@
         <v>228</v>
       </c>
       <c r="J346" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.2">
@@ -11614,7 +11614,7 @@
         <v>228</v>
       </c>
       <c r="J347" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.2">
@@ -11637,7 +11637,7 @@
         <v>225</v>
       </c>
       <c r="J348" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.2">
@@ -11669,7 +11669,7 @@
         <v>228</v>
       </c>
       <c r="J349" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.2">
@@ -11788,7 +11788,7 @@
         <v>225</v>
       </c>
       <c r="J353" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.2">
@@ -11820,7 +11820,7 @@
         <v>223</v>
       </c>
       <c r="J354" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.2">
@@ -11852,7 +11852,7 @@
         <v>233</v>
       </c>
       <c r="J355" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="356" spans="1:10" x14ac:dyDescent="0.2">
@@ -11884,7 +11884,7 @@
         <v>228</v>
       </c>
       <c r="J356" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.2">
@@ -11910,7 +11910,7 @@
         <v>225</v>
       </c>
       <c r="J357" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="358" spans="1:10" x14ac:dyDescent="0.2">
@@ -11936,7 +11936,7 @@
         <v>225</v>
       </c>
       <c r="J358" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.2">
@@ -11968,7 +11968,7 @@
         <v>223</v>
       </c>
       <c r="J359" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.2">
@@ -12000,7 +12000,7 @@
         <v>223</v>
       </c>
       <c r="J360" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.2">
@@ -12032,7 +12032,7 @@
         <v>223</v>
       </c>
       <c r="J361" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.2">
@@ -12064,7 +12064,7 @@
         <v>223</v>
       </c>
       <c r="J362" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.2">
@@ -12186,7 +12186,7 @@
         <v>225</v>
       </c>
       <c r="J366" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="367" spans="1:10" x14ac:dyDescent="0.2">
@@ -12209,7 +12209,7 @@
         <v>225</v>
       </c>
       <c r="J367" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="368" spans="1:10" x14ac:dyDescent="0.2">
@@ -12232,7 +12232,7 @@
         <v>228</v>
       </c>
       <c r="J368" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.2">
@@ -12644,7 +12644,7 @@
         <v>225</v>
       </c>
       <c r="J382" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="383" spans="1:10" x14ac:dyDescent="0.2">
@@ -12734,7 +12734,7 @@
         <v>225</v>
       </c>
       <c r="J385" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="386" spans="1:10" x14ac:dyDescent="0.2">
@@ -12766,7 +12766,7 @@
         <v>223</v>
       </c>
       <c r="J386" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="387" spans="1:10" x14ac:dyDescent="0.2">
@@ -12888,7 +12888,7 @@
         <v>223</v>
       </c>
       <c r="J390" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="391" spans="1:10" x14ac:dyDescent="0.2">
@@ -13437,7 +13437,7 @@
         <v>228</v>
       </c>
       <c r="J408" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="409" spans="1:10" x14ac:dyDescent="0.2">
@@ -13460,7 +13460,7 @@
         <v>227</v>
       </c>
       <c r="J409" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="410" spans="1:10" x14ac:dyDescent="0.2">
@@ -13483,7 +13483,7 @@
         <v>227</v>
       </c>
       <c r="J410" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="411" spans="1:10" x14ac:dyDescent="0.2">
@@ -13730,7 +13730,7 @@
         <v>225</v>
       </c>
       <c r="J418" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="419" spans="1:10" x14ac:dyDescent="0.2">
@@ -13753,7 +13753,7 @@
         <v>225</v>
       </c>
       <c r="J419" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="420" spans="1:10" x14ac:dyDescent="0.2">
@@ -13776,7 +13776,7 @@
         <v>228</v>
       </c>
       <c r="J420" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="421" spans="1:10" x14ac:dyDescent="0.2">
@@ -14174,7 +14174,7 @@
         <v>232</v>
       </c>
       <c r="J433" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="434" spans="1:10" x14ac:dyDescent="0.2">
@@ -14232,7 +14232,7 @@
         <v>232</v>
       </c>
       <c r="J435" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="436" spans="1:10" x14ac:dyDescent="0.2">
@@ -14264,7 +14264,7 @@
         <v>227</v>
       </c>
       <c r="J436" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="437" spans="1:10" x14ac:dyDescent="0.2">
@@ -14351,7 +14351,7 @@
         <v>227</v>
       </c>
       <c r="J439" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="440" spans="1:10" x14ac:dyDescent="0.2">
@@ -14374,7 +14374,7 @@
         <v>224</v>
       </c>
       <c r="J440" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="441" spans="1:10" x14ac:dyDescent="0.2">
@@ -15242,7 +15242,7 @@
         <v>227</v>
       </c>
       <c r="J469" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="470" spans="1:10" x14ac:dyDescent="0.2">
@@ -15268,7 +15268,7 @@
         <v>231</v>
       </c>
       <c r="J470" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="471" spans="1:10" x14ac:dyDescent="0.2">
@@ -15358,7 +15358,7 @@
         <v>227</v>
       </c>
       <c r="J473" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="474" spans="1:10" x14ac:dyDescent="0.2">
@@ -15413,7 +15413,7 @@
         <v>228</v>
       </c>
       <c r="J475" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="476" spans="1:10" x14ac:dyDescent="0.2">
@@ -15436,7 +15436,7 @@
         <v>227</v>
       </c>
       <c r="J476" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="477" spans="1:10" x14ac:dyDescent="0.2">
@@ -15500,7 +15500,7 @@
         <v>225</v>
       </c>
       <c r="J478" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="479" spans="1:10" x14ac:dyDescent="0.2">
@@ -15532,7 +15532,7 @@
         <v>225</v>
       </c>
       <c r="J479" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="480" spans="1:10" x14ac:dyDescent="0.2">
@@ -15564,7 +15564,7 @@
         <v>229</v>
       </c>
       <c r="J480" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="481" spans="1:10" x14ac:dyDescent="0.2">
@@ -15590,7 +15590,7 @@
         <v>225</v>
       </c>
       <c r="J481" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="482" spans="1:10" x14ac:dyDescent="0.2">
@@ -15616,7 +15616,7 @@
         <v>225</v>
       </c>
       <c r="J482" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="483" spans="1:10" x14ac:dyDescent="0.2">
@@ -15648,7 +15648,7 @@
         <v>227</v>
       </c>
       <c r="J483" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="484" spans="1:10" x14ac:dyDescent="0.2">
@@ -15735,7 +15735,7 @@
         <v>231</v>
       </c>
       <c r="J486" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="487" spans="1:10" x14ac:dyDescent="0.2">
@@ -15758,7 +15758,7 @@
         <v>227</v>
       </c>
       <c r="J487" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="488" spans="1:10" x14ac:dyDescent="0.2">
@@ -16170,7 +16170,7 @@
         <v>225</v>
       </c>
       <c r="J501" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="502" spans="1:10" x14ac:dyDescent="0.2">
@@ -16408,7 +16408,7 @@
         <v>228</v>
       </c>
       <c r="J509" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="510" spans="1:10" x14ac:dyDescent="0.2">
@@ -16463,7 +16463,7 @@
         <v>228</v>
       </c>
       <c r="J511" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="512" spans="1:10" x14ac:dyDescent="0.2">
@@ -16486,7 +16486,7 @@
         <v>228</v>
       </c>
       <c r="J512" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="513" spans="1:10" x14ac:dyDescent="0.2">
@@ -16582,7 +16582,7 @@
         <v>223</v>
       </c>
       <c r="J515" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="516" spans="1:10" x14ac:dyDescent="0.2">
@@ -16628,7 +16628,7 @@
         <v>225</v>
       </c>
       <c r="J517" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="518" spans="1:10" x14ac:dyDescent="0.2">
@@ -16747,7 +16747,7 @@
         <v>228</v>
       </c>
       <c r="J521" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="522" spans="1:10" x14ac:dyDescent="0.2">
@@ -16770,7 +16770,7 @@
         <v>228</v>
       </c>
       <c r="J522" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="523" spans="1:10" x14ac:dyDescent="0.2">
@@ -16793,7 +16793,7 @@
         <v>228</v>
       </c>
       <c r="J523" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="524" spans="1:10" x14ac:dyDescent="0.2">
@@ -16967,7 +16967,7 @@
         <v>234</v>
       </c>
       <c r="J529" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="530" spans="1:10" x14ac:dyDescent="0.2">
@@ -17086,7 +17086,7 @@
         <v>227</v>
       </c>
       <c r="J533" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="534" spans="1:10" x14ac:dyDescent="0.2">
@@ -17260,7 +17260,7 @@
         <v>225</v>
       </c>
       <c r="J539" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="540" spans="1:10" x14ac:dyDescent="0.2">
@@ -17292,7 +17292,7 @@
         <v>225</v>
       </c>
       <c r="J540" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="541" spans="1:10" x14ac:dyDescent="0.2">
@@ -17324,7 +17324,7 @@
         <v>225</v>
       </c>
       <c r="J541" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="542" spans="1:10" x14ac:dyDescent="0.2">
@@ -17356,7 +17356,7 @@
         <v>225</v>
       </c>
       <c r="J542" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="543" spans="1:10" x14ac:dyDescent="0.2">
@@ -17382,7 +17382,7 @@
         <v>226</v>
       </c>
       <c r="J543" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="544" spans="1:10" x14ac:dyDescent="0.2">
@@ -17408,7 +17408,7 @@
         <v>226</v>
       </c>
       <c r="J544" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="545" spans="1:10" x14ac:dyDescent="0.2">
@@ -17440,7 +17440,7 @@
         <v>225</v>
       </c>
       <c r="J545" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="546" spans="1:10" x14ac:dyDescent="0.2">
@@ -17562,7 +17562,7 @@
         <v>225</v>
       </c>
       <c r="J549" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="550" spans="1:10" x14ac:dyDescent="0.2">
@@ -17658,7 +17658,7 @@
         <v>229</v>
       </c>
       <c r="J552" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="553" spans="1:10" x14ac:dyDescent="0.2">
@@ -17681,7 +17681,7 @@
         <v>228</v>
       </c>
       <c r="J553" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="554" spans="1:10" x14ac:dyDescent="0.2">
@@ -17704,7 +17704,7 @@
         <v>229</v>
       </c>
       <c r="J554" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="555" spans="1:10" x14ac:dyDescent="0.2">
@@ -17736,7 +17736,7 @@
         <v>227</v>
       </c>
       <c r="J555" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="556" spans="1:10" x14ac:dyDescent="0.2">
@@ -17823,7 +17823,7 @@
         <v>228</v>
       </c>
       <c r="J558" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="559" spans="1:10" x14ac:dyDescent="0.2">
@@ -17846,7 +17846,7 @@
         <v>227</v>
       </c>
       <c r="J559" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="560" spans="1:10" x14ac:dyDescent="0.2">
@@ -17878,7 +17878,7 @@
         <v>229</v>
       </c>
       <c r="J560" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="561" spans="1:10" x14ac:dyDescent="0.2">
@@ -17965,7 +17965,7 @@
         <v>228</v>
       </c>
       <c r="J563" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="564" spans="1:10" x14ac:dyDescent="0.2">
@@ -17988,7 +17988,7 @@
         <v>229</v>
       </c>
       <c r="J564" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="565" spans="1:10" x14ac:dyDescent="0.2">
@@ -18084,7 +18084,7 @@
         <v>223</v>
       </c>
       <c r="J567" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="568" spans="1:10" x14ac:dyDescent="0.2">
@@ -18240,7 +18240,7 @@
         <v>227</v>
       </c>
       <c r="J573" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="574" spans="1:10" x14ac:dyDescent="0.2">
@@ -18295,7 +18295,7 @@
         <v>227</v>
       </c>
       <c r="J575" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="576" spans="1:10" x14ac:dyDescent="0.2">
@@ -18318,7 +18318,7 @@
         <v>229</v>
       </c>
       <c r="J576" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="577" spans="1:10" x14ac:dyDescent="0.2">
@@ -18634,7 +18634,7 @@
         <v>227</v>
       </c>
       <c r="J587" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="588" spans="1:10" x14ac:dyDescent="0.2">
@@ -18666,7 +18666,7 @@
         <v>232</v>
       </c>
       <c r="J588" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="589" spans="1:10" x14ac:dyDescent="0.2">
@@ -18698,7 +18698,7 @@
         <v>232</v>
       </c>
       <c r="J589" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="590" spans="1:10" x14ac:dyDescent="0.2">
@@ -18730,7 +18730,7 @@
         <v>227</v>
       </c>
       <c r="J590" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="591" spans="1:10" x14ac:dyDescent="0.2">
@@ -18756,7 +18756,7 @@
         <v>223</v>
       </c>
       <c r="J591" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="592" spans="1:10" x14ac:dyDescent="0.2">
@@ -18788,7 +18788,7 @@
         <v>223</v>
       </c>
       <c r="J592" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="593" spans="1:10" x14ac:dyDescent="0.2">
@@ -18820,7 +18820,7 @@
         <v>223</v>
       </c>
       <c r="J593" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="594" spans="1:10" x14ac:dyDescent="0.2">
@@ -18852,7 +18852,7 @@
         <v>223</v>
       </c>
       <c r="J594" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="595" spans="1:10" x14ac:dyDescent="0.2">
@@ -18884,7 +18884,7 @@
         <v>223</v>
       </c>
       <c r="J595" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="596" spans="1:10" x14ac:dyDescent="0.2">
@@ -18910,7 +18910,7 @@
         <v>223</v>
       </c>
       <c r="J596" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="597" spans="1:10" x14ac:dyDescent="0.2">
@@ -18936,7 +18936,7 @@
         <v>223</v>
       </c>
       <c r="J597" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="598" spans="1:10" x14ac:dyDescent="0.2">
@@ -18962,7 +18962,7 @@
         <v>223</v>
       </c>
       <c r="J598" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="599" spans="1:10" x14ac:dyDescent="0.2">
@@ -19058,7 +19058,7 @@
         <v>225</v>
       </c>
       <c r="J601" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="602" spans="1:10" x14ac:dyDescent="0.2">
@@ -19081,7 +19081,7 @@
         <v>225</v>
       </c>
       <c r="J602" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="603" spans="1:10" x14ac:dyDescent="0.2">
@@ -19104,7 +19104,7 @@
         <v>228</v>
       </c>
       <c r="J603" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="604" spans="1:10" x14ac:dyDescent="0.2">
@@ -19200,7 +19200,7 @@
         <v>225</v>
       </c>
       <c r="J606" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="607" spans="1:10" x14ac:dyDescent="0.2">
@@ -19223,7 +19223,7 @@
         <v>228</v>
       </c>
       <c r="J607" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="608" spans="1:10" x14ac:dyDescent="0.2">
@@ -19246,7 +19246,7 @@
         <v>225</v>
       </c>
       <c r="J608" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="609" spans="1:10" x14ac:dyDescent="0.2">
@@ -19420,7 +19420,7 @@
         <v>226</v>
       </c>
       <c r="J614" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="615" spans="1:10" x14ac:dyDescent="0.2">
@@ -19484,7 +19484,7 @@
         <v>228</v>
       </c>
       <c r="J616" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="617" spans="1:10" x14ac:dyDescent="0.2">
@@ -19507,7 +19507,7 @@
         <v>225</v>
       </c>
       <c r="J617" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="618" spans="1:10" x14ac:dyDescent="0.2">
@@ -19530,7 +19530,7 @@
         <v>225</v>
       </c>
       <c r="J618" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="619" spans="1:10" x14ac:dyDescent="0.2">
@@ -19777,7 +19777,7 @@
         <v>225</v>
       </c>
       <c r="J626" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="627" spans="1:10" x14ac:dyDescent="0.2">
@@ -19800,7 +19800,7 @@
         <v>225</v>
       </c>
       <c r="J627" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="628" spans="1:10" x14ac:dyDescent="0.2">
@@ -19823,7 +19823,7 @@
         <v>228</v>
       </c>
       <c r="J628" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="629" spans="1:10" x14ac:dyDescent="0.2">
@@ -19855,7 +19855,7 @@
         <v>225</v>
       </c>
       <c r="J629" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="630" spans="1:10" x14ac:dyDescent="0.2">
@@ -19942,7 +19942,7 @@
         <v>228</v>
       </c>
       <c r="J632" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="633" spans="1:10" x14ac:dyDescent="0.2">
@@ -19965,7 +19965,7 @@
         <v>225</v>
       </c>
       <c r="J633" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="634" spans="1:10" x14ac:dyDescent="0.2">
@@ -20148,7 +20148,7 @@
         <v>227</v>
       </c>
       <c r="J639" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.2">
@@ -20180,7 +20180,7 @@
         <v>223</v>
       </c>
       <c r="J640" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.2">
@@ -20212,7 +20212,7 @@
         <v>232</v>
       </c>
       <c r="J641" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.2">
@@ -20244,7 +20244,7 @@
         <v>227</v>
       </c>
       <c r="J642" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="643" spans="1:10" x14ac:dyDescent="0.2">
@@ -20270,7 +20270,7 @@
         <v>232</v>
       </c>
       <c r="J643" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="644" spans="1:10" x14ac:dyDescent="0.2">
@@ -20476,7 +20476,7 @@
         <v>229</v>
       </c>
       <c r="J650" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="651" spans="1:10" x14ac:dyDescent="0.2">
@@ -20609,7 +20609,7 @@
         <v>228</v>
       </c>
       <c r="J655" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="656" spans="1:10" x14ac:dyDescent="0.2">
@@ -20673,7 +20673,7 @@
         <v>228</v>
       </c>
       <c r="J657" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="658" spans="1:11" x14ac:dyDescent="0.2">
@@ -20731,7 +20731,7 @@
         <v>229</v>
       </c>
       <c r="J659" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="660" spans="1:11" x14ac:dyDescent="0.2">
@@ -20829,7 +20829,7 @@
         <v>227</v>
       </c>
       <c r="J662" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K662" s="3"/>
     </row>
@@ -20853,7 +20853,7 @@
         <v>227</v>
       </c>
       <c r="J663" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K663" s="3"/>
     </row>
@@ -20877,7 +20877,7 @@
         <v>224</v>
       </c>
       <c r="J664" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K664" s="3"/>
     </row>
@@ -20943,7 +20943,7 @@
         <v>228</v>
       </c>
       <c r="J666" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K666" s="3"/>
     </row>
@@ -21000,7 +21000,7 @@
         <v>228</v>
       </c>
       <c r="J668" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K668" s="3"/>
     </row>
@@ -21024,7 +21024,7 @@
         <v>231</v>
       </c>
       <c r="J669" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K669" s="3"/>
     </row>
@@ -21361,7 +21361,7 @@
         <v>232</v>
       </c>
       <c r="J680" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="681" spans="1:10" x14ac:dyDescent="0.2">
@@ -21457,7 +21457,7 @@
         <v>232</v>
       </c>
       <c r="J683" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="684" spans="1:10" x14ac:dyDescent="0.2">
@@ -22126,7 +22126,7 @@
         <v>225</v>
       </c>
       <c r="J707" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="708" spans="1:10" x14ac:dyDescent="0.2">
@@ -22213,7 +22213,7 @@
         <v>225</v>
       </c>
       <c r="J710" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.2">
@@ -22236,7 +22236,7 @@
         <v>228</v>
       </c>
       <c r="J711" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.2">
@@ -22552,7 +22552,7 @@
         <v>225</v>
       </c>
       <c r="J722" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.2">
@@ -22639,7 +22639,7 @@
         <v>228</v>
       </c>
       <c r="J725" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="726" spans="1:10" x14ac:dyDescent="0.2">
@@ -22662,7 +22662,7 @@
         <v>225</v>
       </c>
       <c r="J726" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="727" spans="1:10" x14ac:dyDescent="0.2">
@@ -22758,7 +22758,7 @@
         <v>227</v>
       </c>
       <c r="J729" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="730" spans="1:10" x14ac:dyDescent="0.2">
@@ -22781,7 +22781,7 @@
         <v>228</v>
       </c>
       <c r="J730" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="731" spans="1:10" x14ac:dyDescent="0.2">
@@ -22804,7 +22804,7 @@
         <v>227</v>
       </c>
       <c r="J731" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Listed out manual corrections to artery_tcl"
This reverts commit 12bdea11a9c4942d3a06e55bbe95421349a33270.
</commit_message>
<xml_diff>
--- a/tmc_qc.xlsx
+++ b/tmc_qc.xlsx
@@ -731,6 +731,9 @@
     <t>Minor Arterial Ramp</t>
   </si>
   <si>
+    <t>change</t>
+  </si>
+  <si>
     <t>Ok</t>
   </si>
   <si>
@@ -1056,9 +1059,6 @@
   </si>
   <si>
     <t>change W to 8128</t>
-  </si>
-  <si>
-    <t>change S to 445260</t>
   </si>
 </sst>
 </file>
@@ -1392,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K731"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E229" sqref="E229:E234"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1436,10 +1436,10 @@
         <v>221</v>
       </c>
       <c r="I1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="J1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1471,7 +1471,7 @@
         <v>224</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1503,7 +1503,7 @@
         <v>223</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1535,7 +1535,7 @@
         <v>225</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1567,7 +1567,7 @@
         <v>226</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1593,7 +1593,7 @@
         <v>225</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1840,7 +1840,7 @@
         <v>226</v>
       </c>
       <c r="J14" t="s">
-        <v>344</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1895,7 +1895,7 @@
         <v>225</v>
       </c>
       <c r="J16" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1927,7 +1927,7 @@
         <v>225</v>
       </c>
       <c r="J17" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -2014,7 +2014,7 @@
         <v>225</v>
       </c>
       <c r="J20" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -2037,7 +2037,7 @@
         <v>229</v>
       </c>
       <c r="J21" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -2394,7 +2394,7 @@
         <v>225</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -2426,7 +2426,7 @@
         <v>225</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -2452,7 +2452,7 @@
         <v>224</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -2478,7 +2478,7 @@
         <v>225</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -2504,7 +2504,7 @@
         <v>224</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -2530,7 +2530,7 @@
         <v>225</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -2626,7 +2626,7 @@
         <v>226</v>
       </c>
       <c r="J41" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -2887,7 +2887,7 @@
         <v>225</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -2919,7 +2919,7 @@
         <v>225</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -2983,7 +2983,7 @@
         <v>225</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -3009,7 +3009,7 @@
         <v>223</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -3224,7 +3224,7 @@
         <v>227</v>
       </c>
       <c r="J61" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -3311,7 +3311,7 @@
         <v>225</v>
       </c>
       <c r="J64" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -3558,7 +3558,7 @@
         <v>229</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -3590,7 +3590,7 @@
         <v>225</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -3642,7 +3642,7 @@
         <v>223</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
@@ -3668,7 +3668,7 @@
         <v>229</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -3772,7 +3772,7 @@
         <v>225</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -4097,7 +4097,7 @@
         <v>223</v>
       </c>
       <c r="J91" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
@@ -4216,7 +4216,7 @@
         <v>225</v>
       </c>
       <c r="J95" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
@@ -4248,7 +4248,7 @@
         <v>225</v>
       </c>
       <c r="J96" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -4280,7 +4280,7 @@
         <v>229</v>
       </c>
       <c r="J97" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
@@ -4367,7 +4367,7 @@
         <v>223</v>
       </c>
       <c r="J100" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -4390,7 +4390,7 @@
         <v>229</v>
       </c>
       <c r="J101" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
@@ -4517,7 +4517,7 @@
         <v>229</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
@@ -4549,7 +4549,7 @@
         <v>225</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
@@ -4581,7 +4581,7 @@
         <v>225</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
@@ -4613,7 +4613,7 @@
         <v>229</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
@@ -4639,7 +4639,7 @@
         <v>225</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -4964,7 +4964,7 @@
         <v>227</v>
       </c>
       <c r="J121" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
@@ -5051,7 +5051,7 @@
         <v>227</v>
       </c>
       <c r="J124" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
@@ -5074,7 +5074,7 @@
         <v>228</v>
       </c>
       <c r="J125" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
@@ -5614,7 +5614,7 @@
         <v>227</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
@@ -5646,7 +5646,7 @@
         <v>225</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
@@ -5672,7 +5672,7 @@
         <v>225</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
@@ -6235,7 +6235,7 @@
         <v>229</v>
       </c>
       <c r="J164" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
@@ -6377,7 +6377,7 @@
         <v>225</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
@@ -6435,7 +6435,7 @@
         <v>225</v>
       </c>
       <c r="J171" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.2">
@@ -6833,7 +6833,7 @@
         <v>225</v>
       </c>
       <c r="J184" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
@@ -6856,7 +6856,7 @@
         <v>225</v>
       </c>
       <c r="J185" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
@@ -6879,7 +6879,7 @@
         <v>228</v>
       </c>
       <c r="J186" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
@@ -6975,7 +6975,7 @@
         <v>225</v>
       </c>
       <c r="J189" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
@@ -7053,7 +7053,7 @@
         <v>225</v>
       </c>
       <c r="J192" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.2">
@@ -7140,7 +7140,7 @@
         <v>230</v>
       </c>
       <c r="J195" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.2">
@@ -7163,7 +7163,7 @@
         <v>225</v>
       </c>
       <c r="J196" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.2">
@@ -7195,7 +7195,7 @@
         <v>228</v>
       </c>
       <c r="J197" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
@@ -7314,7 +7314,7 @@
         <v>225</v>
       </c>
       <c r="J201" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.2">
@@ -7346,7 +7346,7 @@
         <v>225</v>
       </c>
       <c r="J202" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.2">
@@ -7433,7 +7433,7 @@
         <v>228</v>
       </c>
       <c r="J205" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.2">
@@ -7456,7 +7456,7 @@
         <v>225</v>
       </c>
       <c r="J206" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
@@ -8202,7 +8202,7 @@
         <v>225</v>
       </c>
       <c r="J231" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.2">
@@ -8234,7 +8234,7 @@
         <v>227</v>
       </c>
       <c r="J232" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.2">
@@ -8312,7 +8312,7 @@
         <v>225</v>
       </c>
       <c r="J235" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.2">
@@ -8344,7 +8344,7 @@
         <v>227</v>
       </c>
       <c r="J236" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
@@ -8376,7 +8376,7 @@
         <v>227</v>
       </c>
       <c r="J237" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.2">
@@ -8408,7 +8408,7 @@
         <v>225</v>
       </c>
       <c r="J238" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.2">
@@ -8628,7 +8628,7 @@
         <v>227</v>
       </c>
       <c r="J246" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.2">
@@ -8724,7 +8724,7 @@
         <v>225</v>
       </c>
       <c r="J249" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.2">
@@ -8747,7 +8747,7 @@
         <v>228</v>
       </c>
       <c r="J250" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.2">
@@ -8770,7 +8770,7 @@
         <v>225</v>
       </c>
       <c r="J251" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">
@@ -8834,7 +8834,7 @@
         <v>226</v>
       </c>
       <c r="J253" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.2">
@@ -8924,7 +8924,7 @@
         <v>226</v>
       </c>
       <c r="J256" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.2">
@@ -8988,7 +8988,7 @@
         <v>225</v>
       </c>
       <c r="J258" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.2">
@@ -9043,7 +9043,7 @@
         <v>228</v>
       </c>
       <c r="J260" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.2">
@@ -9066,7 +9066,7 @@
         <v>225</v>
       </c>
       <c r="J261" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.2">
@@ -9130,7 +9130,7 @@
         <v>223</v>
       </c>
       <c r="J263" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.2">
@@ -9220,7 +9220,7 @@
         <v>223</v>
       </c>
       <c r="J266" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.2">
@@ -9403,7 +9403,7 @@
         <v>225</v>
       </c>
       <c r="J272" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.2">
@@ -9435,7 +9435,7 @@
         <v>227</v>
       </c>
       <c r="J273" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.2">
@@ -9467,7 +9467,7 @@
         <v>227</v>
       </c>
       <c r="J274" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.2">
@@ -9499,7 +9499,7 @@
         <v>225</v>
       </c>
       <c r="J275" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.2">
@@ -9525,7 +9525,7 @@
         <v>223</v>
       </c>
       <c r="J276" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.2">
@@ -9653,7 +9653,7 @@
         <v>225</v>
       </c>
       <c r="J280" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.2">
@@ -9679,7 +9679,7 @@
         <v>223</v>
       </c>
       <c r="J281" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.2">
@@ -10004,7 +10004,7 @@
         <v>225</v>
       </c>
       <c r="J292" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.2">
@@ -10091,7 +10091,7 @@
         <v>228</v>
       </c>
       <c r="J295" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
@@ -10114,7 +10114,7 @@
         <v>225</v>
       </c>
       <c r="J296" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.2">
@@ -10146,7 +10146,7 @@
         <v>225</v>
       </c>
       <c r="J297" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.2">
@@ -10233,7 +10233,7 @@
         <v>225</v>
       </c>
       <c r="J300" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.2">
@@ -10256,7 +10256,7 @@
         <v>224</v>
       </c>
       <c r="J301" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.2">
@@ -10471,7 +10471,7 @@
         <v>223</v>
       </c>
       <c r="J308" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.2">
@@ -10561,7 +10561,7 @@
         <v>223</v>
       </c>
       <c r="J311" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.2">
@@ -10776,7 +10776,7 @@
         <v>225</v>
       </c>
       <c r="J318" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.2">
@@ -10808,7 +10808,7 @@
         <v>225</v>
       </c>
       <c r="J319" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.2">
@@ -10840,7 +10840,7 @@
         <v>225</v>
       </c>
       <c r="J320" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.2">
@@ -10866,7 +10866,7 @@
         <v>225</v>
       </c>
       <c r="J321" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.2">
@@ -10892,7 +10892,7 @@
         <v>225</v>
       </c>
       <c r="J322" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.2">
@@ -10918,7 +10918,7 @@
         <v>225</v>
       </c>
       <c r="J323" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.2">
@@ -10982,7 +10982,7 @@
         <v>232</v>
       </c>
       <c r="J325" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.2">
@@ -11124,7 +11124,7 @@
         <v>232</v>
       </c>
       <c r="J330" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.2">
@@ -11449,7 +11449,7 @@
         <v>225</v>
       </c>
       <c r="J341" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.2">
@@ -11472,7 +11472,7 @@
         <v>225</v>
       </c>
       <c r="J342" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.2">
@@ -11495,7 +11495,7 @@
         <v>229</v>
       </c>
       <c r="J343" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.2">
@@ -11527,7 +11527,7 @@
         <v>225</v>
       </c>
       <c r="J344" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="345" spans="1:10" x14ac:dyDescent="0.2">
@@ -11559,7 +11559,7 @@
         <v>225</v>
       </c>
       <c r="J345" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="346" spans="1:10" x14ac:dyDescent="0.2">
@@ -11591,7 +11591,7 @@
         <v>228</v>
       </c>
       <c r="J346" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.2">
@@ -11614,7 +11614,7 @@
         <v>228</v>
       </c>
       <c r="J347" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.2">
@@ -11637,7 +11637,7 @@
         <v>225</v>
       </c>
       <c r="J348" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.2">
@@ -11669,7 +11669,7 @@
         <v>228</v>
       </c>
       <c r="J349" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.2">
@@ -11788,7 +11788,7 @@
         <v>225</v>
       </c>
       <c r="J353" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.2">
@@ -11820,7 +11820,7 @@
         <v>223</v>
       </c>
       <c r="J354" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.2">
@@ -11852,7 +11852,7 @@
         <v>233</v>
       </c>
       <c r="J355" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="356" spans="1:10" x14ac:dyDescent="0.2">
@@ -11884,7 +11884,7 @@
         <v>228</v>
       </c>
       <c r="J356" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.2">
@@ -11910,7 +11910,7 @@
         <v>225</v>
       </c>
       <c r="J357" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="358" spans="1:10" x14ac:dyDescent="0.2">
@@ -11936,7 +11936,7 @@
         <v>225</v>
       </c>
       <c r="J358" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.2">
@@ -11968,7 +11968,7 @@
         <v>223</v>
       </c>
       <c r="J359" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.2">
@@ -12000,7 +12000,7 @@
         <v>223</v>
       </c>
       <c r="J360" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.2">
@@ -12032,7 +12032,7 @@
         <v>223</v>
       </c>
       <c r="J361" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.2">
@@ -12064,7 +12064,7 @@
         <v>223</v>
       </c>
       <c r="J362" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.2">
@@ -12186,7 +12186,7 @@
         <v>225</v>
       </c>
       <c r="J366" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="367" spans="1:10" x14ac:dyDescent="0.2">
@@ -12209,7 +12209,7 @@
         <v>225</v>
       </c>
       <c r="J367" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="368" spans="1:10" x14ac:dyDescent="0.2">
@@ -12232,7 +12232,7 @@
         <v>228</v>
       </c>
       <c r="J368" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.2">
@@ -12644,7 +12644,7 @@
         <v>225</v>
       </c>
       <c r="J382" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="383" spans="1:10" x14ac:dyDescent="0.2">
@@ -12734,7 +12734,7 @@
         <v>225</v>
       </c>
       <c r="J385" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="386" spans="1:10" x14ac:dyDescent="0.2">
@@ -12766,7 +12766,7 @@
         <v>223</v>
       </c>
       <c r="J386" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="387" spans="1:10" x14ac:dyDescent="0.2">
@@ -12888,7 +12888,7 @@
         <v>223</v>
       </c>
       <c r="J390" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="391" spans="1:10" x14ac:dyDescent="0.2">
@@ -13437,7 +13437,7 @@
         <v>228</v>
       </c>
       <c r="J408" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="409" spans="1:10" x14ac:dyDescent="0.2">
@@ -13460,7 +13460,7 @@
         <v>227</v>
       </c>
       <c r="J409" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="410" spans="1:10" x14ac:dyDescent="0.2">
@@ -13483,7 +13483,7 @@
         <v>227</v>
       </c>
       <c r="J410" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="411" spans="1:10" x14ac:dyDescent="0.2">
@@ -13730,7 +13730,7 @@
         <v>225</v>
       </c>
       <c r="J418" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="419" spans="1:10" x14ac:dyDescent="0.2">
@@ -13753,7 +13753,7 @@
         <v>225</v>
       </c>
       <c r="J419" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="420" spans="1:10" x14ac:dyDescent="0.2">
@@ -13776,7 +13776,7 @@
         <v>228</v>
       </c>
       <c r="J420" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="421" spans="1:10" x14ac:dyDescent="0.2">
@@ -14174,7 +14174,7 @@
         <v>232</v>
       </c>
       <c r="J433" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="434" spans="1:10" x14ac:dyDescent="0.2">
@@ -14232,7 +14232,7 @@
         <v>232</v>
       </c>
       <c r="J435" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="436" spans="1:10" x14ac:dyDescent="0.2">
@@ -14264,7 +14264,7 @@
         <v>227</v>
       </c>
       <c r="J436" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="437" spans="1:10" x14ac:dyDescent="0.2">
@@ -14351,7 +14351,7 @@
         <v>227</v>
       </c>
       <c r="J439" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="440" spans="1:10" x14ac:dyDescent="0.2">
@@ -14374,7 +14374,7 @@
         <v>224</v>
       </c>
       <c r="J440" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="441" spans="1:10" x14ac:dyDescent="0.2">
@@ -15242,7 +15242,7 @@
         <v>227</v>
       </c>
       <c r="J469" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="470" spans="1:10" x14ac:dyDescent="0.2">
@@ -15268,7 +15268,7 @@
         <v>231</v>
       </c>
       <c r="J470" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="471" spans="1:10" x14ac:dyDescent="0.2">
@@ -15358,7 +15358,7 @@
         <v>227</v>
       </c>
       <c r="J473" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="474" spans="1:10" x14ac:dyDescent="0.2">
@@ -15413,7 +15413,7 @@
         <v>228</v>
       </c>
       <c r="J475" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="476" spans="1:10" x14ac:dyDescent="0.2">
@@ -15436,7 +15436,7 @@
         <v>227</v>
       </c>
       <c r="J476" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="477" spans="1:10" x14ac:dyDescent="0.2">
@@ -15500,7 +15500,7 @@
         <v>225</v>
       </c>
       <c r="J478" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="479" spans="1:10" x14ac:dyDescent="0.2">
@@ -15532,7 +15532,7 @@
         <v>225</v>
       </c>
       <c r="J479" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="480" spans="1:10" x14ac:dyDescent="0.2">
@@ -15564,7 +15564,7 @@
         <v>229</v>
       </c>
       <c r="J480" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="481" spans="1:10" x14ac:dyDescent="0.2">
@@ -15590,7 +15590,7 @@
         <v>225</v>
       </c>
       <c r="J481" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="482" spans="1:10" x14ac:dyDescent="0.2">
@@ -15616,7 +15616,7 @@
         <v>225</v>
       </c>
       <c r="J482" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="483" spans="1:10" x14ac:dyDescent="0.2">
@@ -15648,7 +15648,7 @@
         <v>227</v>
       </c>
       <c r="J483" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="484" spans="1:10" x14ac:dyDescent="0.2">
@@ -15735,7 +15735,7 @@
         <v>231</v>
       </c>
       <c r="J486" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="487" spans="1:10" x14ac:dyDescent="0.2">
@@ -15758,7 +15758,7 @@
         <v>227</v>
       </c>
       <c r="J487" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="488" spans="1:10" x14ac:dyDescent="0.2">
@@ -16170,7 +16170,7 @@
         <v>225</v>
       </c>
       <c r="J501" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="502" spans="1:10" x14ac:dyDescent="0.2">
@@ -16408,7 +16408,7 @@
         <v>228</v>
       </c>
       <c r="J509" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="510" spans="1:10" x14ac:dyDescent="0.2">
@@ -16463,7 +16463,7 @@
         <v>228</v>
       </c>
       <c r="J511" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="512" spans="1:10" x14ac:dyDescent="0.2">
@@ -16486,7 +16486,7 @@
         <v>228</v>
       </c>
       <c r="J512" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="513" spans="1:10" x14ac:dyDescent="0.2">
@@ -16582,7 +16582,7 @@
         <v>223</v>
       </c>
       <c r="J515" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="516" spans="1:10" x14ac:dyDescent="0.2">
@@ -16628,7 +16628,7 @@
         <v>225</v>
       </c>
       <c r="J517" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="518" spans="1:10" x14ac:dyDescent="0.2">
@@ -16747,7 +16747,7 @@
         <v>228</v>
       </c>
       <c r="J521" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="522" spans="1:10" x14ac:dyDescent="0.2">
@@ -16770,7 +16770,7 @@
         <v>228</v>
       </c>
       <c r="J522" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="523" spans="1:10" x14ac:dyDescent="0.2">
@@ -16793,7 +16793,7 @@
         <v>228</v>
       </c>
       <c r="J523" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="524" spans="1:10" x14ac:dyDescent="0.2">
@@ -16967,7 +16967,7 @@
         <v>234</v>
       </c>
       <c r="J529" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="530" spans="1:10" x14ac:dyDescent="0.2">
@@ -17086,7 +17086,7 @@
         <v>227</v>
       </c>
       <c r="J533" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="534" spans="1:10" x14ac:dyDescent="0.2">
@@ -17260,7 +17260,7 @@
         <v>225</v>
       </c>
       <c r="J539" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="540" spans="1:10" x14ac:dyDescent="0.2">
@@ -17292,7 +17292,7 @@
         <v>225</v>
       </c>
       <c r="J540" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="541" spans="1:10" x14ac:dyDescent="0.2">
@@ -17324,7 +17324,7 @@
         <v>225</v>
       </c>
       <c r="J541" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="542" spans="1:10" x14ac:dyDescent="0.2">
@@ -17356,7 +17356,7 @@
         <v>225</v>
       </c>
       <c r="J542" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="543" spans="1:10" x14ac:dyDescent="0.2">
@@ -17382,7 +17382,7 @@
         <v>226</v>
       </c>
       <c r="J543" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="544" spans="1:10" x14ac:dyDescent="0.2">
@@ -17408,7 +17408,7 @@
         <v>226</v>
       </c>
       <c r="J544" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="545" spans="1:10" x14ac:dyDescent="0.2">
@@ -17440,7 +17440,7 @@
         <v>225</v>
       </c>
       <c r="J545" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="546" spans="1:10" x14ac:dyDescent="0.2">
@@ -17562,7 +17562,7 @@
         <v>225</v>
       </c>
       <c r="J549" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="550" spans="1:10" x14ac:dyDescent="0.2">
@@ -17658,7 +17658,7 @@
         <v>229</v>
       </c>
       <c r="J552" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="553" spans="1:10" x14ac:dyDescent="0.2">
@@ -17681,7 +17681,7 @@
         <v>228</v>
       </c>
       <c r="J553" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="554" spans="1:10" x14ac:dyDescent="0.2">
@@ -17704,7 +17704,7 @@
         <v>229</v>
       </c>
       <c r="J554" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="555" spans="1:10" x14ac:dyDescent="0.2">
@@ -17736,7 +17736,7 @@
         <v>227</v>
       </c>
       <c r="J555" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="556" spans="1:10" x14ac:dyDescent="0.2">
@@ -17823,7 +17823,7 @@
         <v>228</v>
       </c>
       <c r="J558" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="559" spans="1:10" x14ac:dyDescent="0.2">
@@ -17846,7 +17846,7 @@
         <v>227</v>
       </c>
       <c r="J559" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="560" spans="1:10" x14ac:dyDescent="0.2">
@@ -17878,7 +17878,7 @@
         <v>229</v>
       </c>
       <c r="J560" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="561" spans="1:10" x14ac:dyDescent="0.2">
@@ -17965,7 +17965,7 @@
         <v>228</v>
       </c>
       <c r="J563" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="564" spans="1:10" x14ac:dyDescent="0.2">
@@ -17988,7 +17988,7 @@
         <v>229</v>
       </c>
       <c r="J564" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="565" spans="1:10" x14ac:dyDescent="0.2">
@@ -18084,7 +18084,7 @@
         <v>223</v>
       </c>
       <c r="J567" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="568" spans="1:10" x14ac:dyDescent="0.2">
@@ -18240,7 +18240,7 @@
         <v>227</v>
       </c>
       <c r="J573" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="574" spans="1:10" x14ac:dyDescent="0.2">
@@ -18295,7 +18295,7 @@
         <v>227</v>
       </c>
       <c r="J575" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="576" spans="1:10" x14ac:dyDescent="0.2">
@@ -18318,7 +18318,7 @@
         <v>229</v>
       </c>
       <c r="J576" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="577" spans="1:10" x14ac:dyDescent="0.2">
@@ -18634,7 +18634,7 @@
         <v>227</v>
       </c>
       <c r="J587" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="588" spans="1:10" x14ac:dyDescent="0.2">
@@ -18666,7 +18666,7 @@
         <v>232</v>
       </c>
       <c r="J588" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="589" spans="1:10" x14ac:dyDescent="0.2">
@@ -18698,7 +18698,7 @@
         <v>232</v>
       </c>
       <c r="J589" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="590" spans="1:10" x14ac:dyDescent="0.2">
@@ -18730,7 +18730,7 @@
         <v>227</v>
       </c>
       <c r="J590" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="591" spans="1:10" x14ac:dyDescent="0.2">
@@ -18756,7 +18756,7 @@
         <v>223</v>
       </c>
       <c r="J591" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="592" spans="1:10" x14ac:dyDescent="0.2">
@@ -18788,7 +18788,7 @@
         <v>223</v>
       </c>
       <c r="J592" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="593" spans="1:10" x14ac:dyDescent="0.2">
@@ -18820,7 +18820,7 @@
         <v>223</v>
       </c>
       <c r="J593" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="594" spans="1:10" x14ac:dyDescent="0.2">
@@ -18852,7 +18852,7 @@
         <v>223</v>
       </c>
       <c r="J594" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="595" spans="1:10" x14ac:dyDescent="0.2">
@@ -18884,7 +18884,7 @@
         <v>223</v>
       </c>
       <c r="J595" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="596" spans="1:10" x14ac:dyDescent="0.2">
@@ -18910,7 +18910,7 @@
         <v>223</v>
       </c>
       <c r="J596" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="597" spans="1:10" x14ac:dyDescent="0.2">
@@ -18936,7 +18936,7 @@
         <v>223</v>
       </c>
       <c r="J597" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="598" spans="1:10" x14ac:dyDescent="0.2">
@@ -18962,7 +18962,7 @@
         <v>223</v>
       </c>
       <c r="J598" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="599" spans="1:10" x14ac:dyDescent="0.2">
@@ -19058,7 +19058,7 @@
         <v>225</v>
       </c>
       <c r="J601" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="602" spans="1:10" x14ac:dyDescent="0.2">
@@ -19081,7 +19081,7 @@
         <v>225</v>
       </c>
       <c r="J602" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="603" spans="1:10" x14ac:dyDescent="0.2">
@@ -19104,7 +19104,7 @@
         <v>228</v>
       </c>
       <c r="J603" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="604" spans="1:10" x14ac:dyDescent="0.2">
@@ -19200,7 +19200,7 @@
         <v>225</v>
       </c>
       <c r="J606" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="607" spans="1:10" x14ac:dyDescent="0.2">
@@ -19223,7 +19223,7 @@
         <v>228</v>
       </c>
       <c r="J607" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="608" spans="1:10" x14ac:dyDescent="0.2">
@@ -19246,7 +19246,7 @@
         <v>225</v>
       </c>
       <c r="J608" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="609" spans="1:10" x14ac:dyDescent="0.2">
@@ -19420,7 +19420,7 @@
         <v>226</v>
       </c>
       <c r="J614" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="615" spans="1:10" x14ac:dyDescent="0.2">
@@ -19484,7 +19484,7 @@
         <v>228</v>
       </c>
       <c r="J616" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="617" spans="1:10" x14ac:dyDescent="0.2">
@@ -19507,7 +19507,7 @@
         <v>225</v>
       </c>
       <c r="J617" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="618" spans="1:10" x14ac:dyDescent="0.2">
@@ -19530,7 +19530,7 @@
         <v>225</v>
       </c>
       <c r="J618" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="619" spans="1:10" x14ac:dyDescent="0.2">
@@ -19777,7 +19777,7 @@
         <v>225</v>
       </c>
       <c r="J626" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="627" spans="1:10" x14ac:dyDescent="0.2">
@@ -19800,7 +19800,7 @@
         <v>225</v>
       </c>
       <c r="J627" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="628" spans="1:10" x14ac:dyDescent="0.2">
@@ -19823,7 +19823,7 @@
         <v>228</v>
       </c>
       <c r="J628" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="629" spans="1:10" x14ac:dyDescent="0.2">
@@ -19855,7 +19855,7 @@
         <v>225</v>
       </c>
       <c r="J629" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="630" spans="1:10" x14ac:dyDescent="0.2">
@@ -19942,7 +19942,7 @@
         <v>228</v>
       </c>
       <c r="J632" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="633" spans="1:10" x14ac:dyDescent="0.2">
@@ -19965,7 +19965,7 @@
         <v>225</v>
       </c>
       <c r="J633" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="634" spans="1:10" x14ac:dyDescent="0.2">
@@ -20148,7 +20148,7 @@
         <v>227</v>
       </c>
       <c r="J639" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.2">
@@ -20180,7 +20180,7 @@
         <v>223</v>
       </c>
       <c r="J640" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.2">
@@ -20212,7 +20212,7 @@
         <v>232</v>
       </c>
       <c r="J641" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.2">
@@ -20244,7 +20244,7 @@
         <v>227</v>
       </c>
       <c r="J642" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="643" spans="1:10" x14ac:dyDescent="0.2">
@@ -20270,7 +20270,7 @@
         <v>232</v>
       </c>
       <c r="J643" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="644" spans="1:10" x14ac:dyDescent="0.2">
@@ -20476,7 +20476,7 @@
         <v>229</v>
       </c>
       <c r="J650" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="651" spans="1:10" x14ac:dyDescent="0.2">
@@ -20609,7 +20609,7 @@
         <v>228</v>
       </c>
       <c r="J655" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="656" spans="1:10" x14ac:dyDescent="0.2">
@@ -20673,7 +20673,7 @@
         <v>228</v>
       </c>
       <c r="J657" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="658" spans="1:11" x14ac:dyDescent="0.2">
@@ -20731,7 +20731,7 @@
         <v>229</v>
       </c>
       <c r="J659" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="660" spans="1:11" x14ac:dyDescent="0.2">
@@ -20829,7 +20829,7 @@
         <v>227</v>
       </c>
       <c r="J662" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K662" s="3"/>
     </row>
@@ -20853,7 +20853,7 @@
         <v>227</v>
       </c>
       <c r="J663" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K663" s="3"/>
     </row>
@@ -20877,7 +20877,7 @@
         <v>224</v>
       </c>
       <c r="J664" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K664" s="3"/>
     </row>
@@ -20943,7 +20943,7 @@
         <v>228</v>
       </c>
       <c r="J666" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="K666" s="3"/>
     </row>
@@ -21000,7 +21000,7 @@
         <v>228</v>
       </c>
       <c r="J668" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K668" s="3"/>
     </row>
@@ -21024,7 +21024,7 @@
         <v>231</v>
       </c>
       <c r="J669" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K669" s="3"/>
     </row>
@@ -21361,7 +21361,7 @@
         <v>232</v>
       </c>
       <c r="J680" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="681" spans="1:10" x14ac:dyDescent="0.2">
@@ -21457,7 +21457,7 @@
         <v>232</v>
       </c>
       <c r="J683" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="684" spans="1:10" x14ac:dyDescent="0.2">
@@ -22126,7 +22126,7 @@
         <v>225</v>
       </c>
       <c r="J707" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="708" spans="1:10" x14ac:dyDescent="0.2">
@@ -22213,7 +22213,7 @@
         <v>225</v>
       </c>
       <c r="J710" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.2">
@@ -22236,7 +22236,7 @@
         <v>228</v>
       </c>
       <c r="J711" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.2">
@@ -22552,7 +22552,7 @@
         <v>225</v>
       </c>
       <c r="J722" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.2">
@@ -22639,7 +22639,7 @@
         <v>228</v>
       </c>
       <c r="J725" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="726" spans="1:10" x14ac:dyDescent="0.2">
@@ -22662,7 +22662,7 @@
         <v>225</v>
       </c>
       <c r="J726" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="727" spans="1:10" x14ac:dyDescent="0.2">
@@ -22758,7 +22758,7 @@
         <v>227</v>
       </c>
       <c r="J729" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="730" spans="1:10" x14ac:dyDescent="0.2">
@@ -22781,7 +22781,7 @@
         <v>228</v>
       </c>
       <c r="J730" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="731" spans="1:10" x14ac:dyDescent="0.2">
@@ -22804,7 +22804,7 @@
         <v>227</v>
       </c>
       <c r="J731" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Listed out manual corrections to artery_tcl""
This reverts commit 56af8945da1fa165805a09f60e2ba8c525bbbab7.
</commit_message>
<xml_diff>
--- a/tmc_qc.xlsx
+++ b/tmc_qc.xlsx
@@ -731,9 +731,6 @@
     <t>Minor Arterial Ramp</t>
   </si>
   <si>
-    <t>change</t>
-  </si>
-  <si>
     <t>Ok</t>
   </si>
   <si>
@@ -1059,6 +1056,9 @@
   </si>
   <si>
     <t>change W to 8128</t>
+  </si>
+  <si>
+    <t>change S to 445260</t>
   </si>
 </sst>
 </file>
@@ -1392,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K731"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E229" sqref="E229:E234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1436,10 +1436,10 @@
         <v>221</v>
       </c>
       <c r="I1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J1" t="s">
         <v>337</v>
-      </c>
-      <c r="J1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1471,7 +1471,7 @@
         <v>224</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1503,7 +1503,7 @@
         <v>223</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1535,7 +1535,7 @@
         <v>225</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1567,7 +1567,7 @@
         <v>226</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1593,7 +1593,7 @@
         <v>225</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1840,7 +1840,7 @@
         <v>226</v>
       </c>
       <c r="J14" t="s">
-        <v>235</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1895,7 +1895,7 @@
         <v>225</v>
       </c>
       <c r="J16" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1927,7 +1927,7 @@
         <v>225</v>
       </c>
       <c r="J17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -2014,7 +2014,7 @@
         <v>225</v>
       </c>
       <c r="J20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -2037,7 +2037,7 @@
         <v>229</v>
       </c>
       <c r="J21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -2394,7 +2394,7 @@
         <v>225</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -2426,7 +2426,7 @@
         <v>225</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -2452,7 +2452,7 @@
         <v>224</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -2478,7 +2478,7 @@
         <v>225</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -2504,7 +2504,7 @@
         <v>224</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -2530,7 +2530,7 @@
         <v>225</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -2626,7 +2626,7 @@
         <v>226</v>
       </c>
       <c r="J41" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -2887,7 +2887,7 @@
         <v>225</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -2919,7 +2919,7 @@
         <v>225</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -2983,7 +2983,7 @@
         <v>225</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -3009,7 +3009,7 @@
         <v>223</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -3224,7 +3224,7 @@
         <v>227</v>
       </c>
       <c r="J61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -3311,7 +3311,7 @@
         <v>225</v>
       </c>
       <c r="J64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -3558,7 +3558,7 @@
         <v>229</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -3590,7 +3590,7 @@
         <v>225</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -3642,7 +3642,7 @@
         <v>223</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
@@ -3668,7 +3668,7 @@
         <v>229</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -3772,7 +3772,7 @@
         <v>225</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -4097,7 +4097,7 @@
         <v>223</v>
       </c>
       <c r="J91" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
@@ -4216,7 +4216,7 @@
         <v>225</v>
       </c>
       <c r="J95" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
@@ -4248,7 +4248,7 @@
         <v>225</v>
       </c>
       <c r="J96" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -4280,7 +4280,7 @@
         <v>229</v>
       </c>
       <c r="J97" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
@@ -4367,7 +4367,7 @@
         <v>223</v>
       </c>
       <c r="J100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -4390,7 +4390,7 @@
         <v>229</v>
       </c>
       <c r="J101" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
@@ -4517,7 +4517,7 @@
         <v>229</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
@@ -4549,7 +4549,7 @@
         <v>225</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
@@ -4581,7 +4581,7 @@
         <v>225</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
@@ -4613,7 +4613,7 @@
         <v>229</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
@@ -4639,7 +4639,7 @@
         <v>225</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -4964,7 +4964,7 @@
         <v>227</v>
       </c>
       <c r="J121" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
@@ -5051,7 +5051,7 @@
         <v>227</v>
       </c>
       <c r="J124" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
@@ -5074,7 +5074,7 @@
         <v>228</v>
       </c>
       <c r="J125" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
@@ -5614,7 +5614,7 @@
         <v>227</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
@@ -5646,7 +5646,7 @@
         <v>225</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
@@ -5672,7 +5672,7 @@
         <v>225</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
@@ -6235,7 +6235,7 @@
         <v>229</v>
       </c>
       <c r="J164" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
@@ -6377,7 +6377,7 @@
         <v>225</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
@@ -6435,7 +6435,7 @@
         <v>225</v>
       </c>
       <c r="J171" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.2">
@@ -6833,7 +6833,7 @@
         <v>225</v>
       </c>
       <c r="J184" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
@@ -6856,7 +6856,7 @@
         <v>225</v>
       </c>
       <c r="J185" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
@@ -6879,7 +6879,7 @@
         <v>228</v>
       </c>
       <c r="J186" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
@@ -6975,7 +6975,7 @@
         <v>225</v>
       </c>
       <c r="J189" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
@@ -7053,7 +7053,7 @@
         <v>225</v>
       </c>
       <c r="J192" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.2">
@@ -7140,7 +7140,7 @@
         <v>230</v>
       </c>
       <c r="J195" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.2">
@@ -7163,7 +7163,7 @@
         <v>225</v>
       </c>
       <c r="J196" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.2">
@@ -7195,7 +7195,7 @@
         <v>228</v>
       </c>
       <c r="J197" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
@@ -7314,7 +7314,7 @@
         <v>225</v>
       </c>
       <c r="J201" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.2">
@@ -7346,7 +7346,7 @@
         <v>225</v>
       </c>
       <c r="J202" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.2">
@@ -7433,7 +7433,7 @@
         <v>228</v>
       </c>
       <c r="J205" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.2">
@@ -7456,7 +7456,7 @@
         <v>225</v>
       </c>
       <c r="J206" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
@@ -8202,7 +8202,7 @@
         <v>225</v>
       </c>
       <c r="J231" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.2">
@@ -8234,7 +8234,7 @@
         <v>227</v>
       </c>
       <c r="J232" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.2">
@@ -8312,7 +8312,7 @@
         <v>225</v>
       </c>
       <c r="J235" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.2">
@@ -8344,7 +8344,7 @@
         <v>227</v>
       </c>
       <c r="J236" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
@@ -8376,7 +8376,7 @@
         <v>227</v>
       </c>
       <c r="J237" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.2">
@@ -8408,7 +8408,7 @@
         <v>225</v>
       </c>
       <c r="J238" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.2">
@@ -8628,7 +8628,7 @@
         <v>227</v>
       </c>
       <c r="J246" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.2">
@@ -8724,7 +8724,7 @@
         <v>225</v>
       </c>
       <c r="J249" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.2">
@@ -8747,7 +8747,7 @@
         <v>228</v>
       </c>
       <c r="J250" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.2">
@@ -8770,7 +8770,7 @@
         <v>225</v>
       </c>
       <c r="J251" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.2">
@@ -8834,7 +8834,7 @@
         <v>226</v>
       </c>
       <c r="J253" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.2">
@@ -8924,7 +8924,7 @@
         <v>226</v>
       </c>
       <c r="J256" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.2">
@@ -8988,7 +8988,7 @@
         <v>225</v>
       </c>
       <c r="J258" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.2">
@@ -9043,7 +9043,7 @@
         <v>228</v>
       </c>
       <c r="J260" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.2">
@@ -9066,7 +9066,7 @@
         <v>225</v>
       </c>
       <c r="J261" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.2">
@@ -9130,7 +9130,7 @@
         <v>223</v>
       </c>
       <c r="J263" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.2">
@@ -9220,7 +9220,7 @@
         <v>223</v>
       </c>
       <c r="J266" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.2">
@@ -9403,7 +9403,7 @@
         <v>225</v>
       </c>
       <c r="J272" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.2">
@@ -9435,7 +9435,7 @@
         <v>227</v>
       </c>
       <c r="J273" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.2">
@@ -9467,7 +9467,7 @@
         <v>227</v>
       </c>
       <c r="J274" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.2">
@@ -9499,7 +9499,7 @@
         <v>225</v>
       </c>
       <c r="J275" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.2">
@@ -9525,7 +9525,7 @@
         <v>223</v>
       </c>
       <c r="J276" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.2">
@@ -9653,7 +9653,7 @@
         <v>225</v>
       </c>
       <c r="J280" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.2">
@@ -9679,7 +9679,7 @@
         <v>223</v>
       </c>
       <c r="J281" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.2">
@@ -10004,7 +10004,7 @@
         <v>225</v>
       </c>
       <c r="J292" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.2">
@@ -10091,7 +10091,7 @@
         <v>228</v>
       </c>
       <c r="J295" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
@@ -10114,7 +10114,7 @@
         <v>225</v>
       </c>
       <c r="J296" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.2">
@@ -10146,7 +10146,7 @@
         <v>225</v>
       </c>
       <c r="J297" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.2">
@@ -10233,7 +10233,7 @@
         <v>225</v>
       </c>
       <c r="J300" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.2">
@@ -10256,7 +10256,7 @@
         <v>224</v>
       </c>
       <c r="J301" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.2">
@@ -10471,7 +10471,7 @@
         <v>223</v>
       </c>
       <c r="J308" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.2">
@@ -10561,7 +10561,7 @@
         <v>223</v>
       </c>
       <c r="J311" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.2">
@@ -10776,7 +10776,7 @@
         <v>225</v>
       </c>
       <c r="J318" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.2">
@@ -10808,7 +10808,7 @@
         <v>225</v>
       </c>
       <c r="J319" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.2">
@@ -10840,7 +10840,7 @@
         <v>225</v>
       </c>
       <c r="J320" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.2">
@@ -10866,7 +10866,7 @@
         <v>225</v>
       </c>
       <c r="J321" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.2">
@@ -10892,7 +10892,7 @@
         <v>225</v>
       </c>
       <c r="J322" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.2">
@@ -10918,7 +10918,7 @@
         <v>225</v>
       </c>
       <c r="J323" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.2">
@@ -10982,7 +10982,7 @@
         <v>232</v>
       </c>
       <c r="J325" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.2">
@@ -11124,7 +11124,7 @@
         <v>232</v>
       </c>
       <c r="J330" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.2">
@@ -11449,7 +11449,7 @@
         <v>225</v>
       </c>
       <c r="J341" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.2">
@@ -11472,7 +11472,7 @@
         <v>225</v>
       </c>
       <c r="J342" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.2">
@@ -11495,7 +11495,7 @@
         <v>229</v>
       </c>
       <c r="J343" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.2">
@@ -11527,7 +11527,7 @@
         <v>225</v>
       </c>
       <c r="J344" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="345" spans="1:10" x14ac:dyDescent="0.2">
@@ -11559,7 +11559,7 @@
         <v>225</v>
       </c>
       <c r="J345" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="346" spans="1:10" x14ac:dyDescent="0.2">
@@ -11591,7 +11591,7 @@
         <v>228</v>
       </c>
       <c r="J346" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.2">
@@ -11614,7 +11614,7 @@
         <v>228</v>
       </c>
       <c r="J347" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.2">
@@ -11637,7 +11637,7 @@
         <v>225</v>
       </c>
       <c r="J348" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.2">
@@ -11669,7 +11669,7 @@
         <v>228</v>
       </c>
       <c r="J349" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.2">
@@ -11788,7 +11788,7 @@
         <v>225</v>
       </c>
       <c r="J353" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.2">
@@ -11820,7 +11820,7 @@
         <v>223</v>
       </c>
       <c r="J354" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.2">
@@ -11852,7 +11852,7 @@
         <v>233</v>
       </c>
       <c r="J355" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="356" spans="1:10" x14ac:dyDescent="0.2">
@@ -11884,7 +11884,7 @@
         <v>228</v>
       </c>
       <c r="J356" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.2">
@@ -11910,7 +11910,7 @@
         <v>225</v>
       </c>
       <c r="J357" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="358" spans="1:10" x14ac:dyDescent="0.2">
@@ -11936,7 +11936,7 @@
         <v>225</v>
       </c>
       <c r="J358" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.2">
@@ -11968,7 +11968,7 @@
         <v>223</v>
       </c>
       <c r="J359" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.2">
@@ -12000,7 +12000,7 @@
         <v>223</v>
       </c>
       <c r="J360" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.2">
@@ -12032,7 +12032,7 @@
         <v>223</v>
       </c>
       <c r="J361" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.2">
@@ -12064,7 +12064,7 @@
         <v>223</v>
       </c>
       <c r="J362" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.2">
@@ -12186,7 +12186,7 @@
         <v>225</v>
       </c>
       <c r="J366" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="367" spans="1:10" x14ac:dyDescent="0.2">
@@ -12209,7 +12209,7 @@
         <v>225</v>
       </c>
       <c r="J367" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="368" spans="1:10" x14ac:dyDescent="0.2">
@@ -12232,7 +12232,7 @@
         <v>228</v>
       </c>
       <c r="J368" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.2">
@@ -12644,7 +12644,7 @@
         <v>225</v>
       </c>
       <c r="J382" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="383" spans="1:10" x14ac:dyDescent="0.2">
@@ -12734,7 +12734,7 @@
         <v>225</v>
       </c>
       <c r="J385" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="386" spans="1:10" x14ac:dyDescent="0.2">
@@ -12766,7 +12766,7 @@
         <v>223</v>
       </c>
       <c r="J386" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="387" spans="1:10" x14ac:dyDescent="0.2">
@@ -12888,7 +12888,7 @@
         <v>223</v>
       </c>
       <c r="J390" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="391" spans="1:10" x14ac:dyDescent="0.2">
@@ -13437,7 +13437,7 @@
         <v>228</v>
       </c>
       <c r="J408" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="409" spans="1:10" x14ac:dyDescent="0.2">
@@ -13460,7 +13460,7 @@
         <v>227</v>
       </c>
       <c r="J409" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="410" spans="1:10" x14ac:dyDescent="0.2">
@@ -13483,7 +13483,7 @@
         <v>227</v>
       </c>
       <c r="J410" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="411" spans="1:10" x14ac:dyDescent="0.2">
@@ -13730,7 +13730,7 @@
         <v>225</v>
       </c>
       <c r="J418" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="419" spans="1:10" x14ac:dyDescent="0.2">
@@ -13753,7 +13753,7 @@
         <v>225</v>
       </c>
       <c r="J419" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="420" spans="1:10" x14ac:dyDescent="0.2">
@@ -13776,7 +13776,7 @@
         <v>228</v>
       </c>
       <c r="J420" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="421" spans="1:10" x14ac:dyDescent="0.2">
@@ -14174,7 +14174,7 @@
         <v>232</v>
       </c>
       <c r="J433" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="434" spans="1:10" x14ac:dyDescent="0.2">
@@ -14232,7 +14232,7 @@
         <v>232</v>
       </c>
       <c r="J435" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="436" spans="1:10" x14ac:dyDescent="0.2">
@@ -14264,7 +14264,7 @@
         <v>227</v>
       </c>
       <c r="J436" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="437" spans="1:10" x14ac:dyDescent="0.2">
@@ -14351,7 +14351,7 @@
         <v>227</v>
       </c>
       <c r="J439" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="440" spans="1:10" x14ac:dyDescent="0.2">
@@ -14374,7 +14374,7 @@
         <v>224</v>
       </c>
       <c r="J440" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="441" spans="1:10" x14ac:dyDescent="0.2">
@@ -15242,7 +15242,7 @@
         <v>227</v>
       </c>
       <c r="J469" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="470" spans="1:10" x14ac:dyDescent="0.2">
@@ -15268,7 +15268,7 @@
         <v>231</v>
       </c>
       <c r="J470" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="471" spans="1:10" x14ac:dyDescent="0.2">
@@ -15358,7 +15358,7 @@
         <v>227</v>
       </c>
       <c r="J473" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="474" spans="1:10" x14ac:dyDescent="0.2">
@@ -15413,7 +15413,7 @@
         <v>228</v>
       </c>
       <c r="J475" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="476" spans="1:10" x14ac:dyDescent="0.2">
@@ -15436,7 +15436,7 @@
         <v>227</v>
       </c>
       <c r="J476" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="477" spans="1:10" x14ac:dyDescent="0.2">
@@ -15500,7 +15500,7 @@
         <v>225</v>
       </c>
       <c r="J478" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="479" spans="1:10" x14ac:dyDescent="0.2">
@@ -15532,7 +15532,7 @@
         <v>225</v>
       </c>
       <c r="J479" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="480" spans="1:10" x14ac:dyDescent="0.2">
@@ -15564,7 +15564,7 @@
         <v>229</v>
       </c>
       <c r="J480" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="481" spans="1:10" x14ac:dyDescent="0.2">
@@ -15590,7 +15590,7 @@
         <v>225</v>
       </c>
       <c r="J481" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="482" spans="1:10" x14ac:dyDescent="0.2">
@@ -15616,7 +15616,7 @@
         <v>225</v>
       </c>
       <c r="J482" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="483" spans="1:10" x14ac:dyDescent="0.2">
@@ -15648,7 +15648,7 @@
         <v>227</v>
       </c>
       <c r="J483" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="484" spans="1:10" x14ac:dyDescent="0.2">
@@ -15735,7 +15735,7 @@
         <v>231</v>
       </c>
       <c r="J486" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="487" spans="1:10" x14ac:dyDescent="0.2">
@@ -15758,7 +15758,7 @@
         <v>227</v>
       </c>
       <c r="J487" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="488" spans="1:10" x14ac:dyDescent="0.2">
@@ -16170,7 +16170,7 @@
         <v>225</v>
       </c>
       <c r="J501" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="502" spans="1:10" x14ac:dyDescent="0.2">
@@ -16408,7 +16408,7 @@
         <v>228</v>
       </c>
       <c r="J509" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="510" spans="1:10" x14ac:dyDescent="0.2">
@@ -16463,7 +16463,7 @@
         <v>228</v>
       </c>
       <c r="J511" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="512" spans="1:10" x14ac:dyDescent="0.2">
@@ -16486,7 +16486,7 @@
         <v>228</v>
       </c>
       <c r="J512" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="513" spans="1:10" x14ac:dyDescent="0.2">
@@ -16582,7 +16582,7 @@
         <v>223</v>
       </c>
       <c r="J515" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="516" spans="1:10" x14ac:dyDescent="0.2">
@@ -16628,7 +16628,7 @@
         <v>225</v>
       </c>
       <c r="J517" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="518" spans="1:10" x14ac:dyDescent="0.2">
@@ -16747,7 +16747,7 @@
         <v>228</v>
       </c>
       <c r="J521" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="522" spans="1:10" x14ac:dyDescent="0.2">
@@ -16770,7 +16770,7 @@
         <v>228</v>
       </c>
       <c r="J522" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="523" spans="1:10" x14ac:dyDescent="0.2">
@@ -16793,7 +16793,7 @@
         <v>228</v>
       </c>
       <c r="J523" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="524" spans="1:10" x14ac:dyDescent="0.2">
@@ -16967,7 +16967,7 @@
         <v>234</v>
       </c>
       <c r="J529" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="530" spans="1:10" x14ac:dyDescent="0.2">
@@ -17086,7 +17086,7 @@
         <v>227</v>
       </c>
       <c r="J533" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="534" spans="1:10" x14ac:dyDescent="0.2">
@@ -17260,7 +17260,7 @@
         <v>225</v>
       </c>
       <c r="J539" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="540" spans="1:10" x14ac:dyDescent="0.2">
@@ -17292,7 +17292,7 @@
         <v>225</v>
       </c>
       <c r="J540" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="541" spans="1:10" x14ac:dyDescent="0.2">
@@ -17324,7 +17324,7 @@
         <v>225</v>
       </c>
       <c r="J541" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="542" spans="1:10" x14ac:dyDescent="0.2">
@@ -17356,7 +17356,7 @@
         <v>225</v>
       </c>
       <c r="J542" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="543" spans="1:10" x14ac:dyDescent="0.2">
@@ -17382,7 +17382,7 @@
         <v>226</v>
       </c>
       <c r="J543" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="544" spans="1:10" x14ac:dyDescent="0.2">
@@ -17408,7 +17408,7 @@
         <v>226</v>
       </c>
       <c r="J544" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="545" spans="1:10" x14ac:dyDescent="0.2">
@@ -17440,7 +17440,7 @@
         <v>225</v>
       </c>
       <c r="J545" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="546" spans="1:10" x14ac:dyDescent="0.2">
@@ -17562,7 +17562,7 @@
         <v>225</v>
       </c>
       <c r="J549" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="550" spans="1:10" x14ac:dyDescent="0.2">
@@ -17658,7 +17658,7 @@
         <v>229</v>
       </c>
       <c r="J552" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="553" spans="1:10" x14ac:dyDescent="0.2">
@@ -17681,7 +17681,7 @@
         <v>228</v>
       </c>
       <c r="J553" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="554" spans="1:10" x14ac:dyDescent="0.2">
@@ -17704,7 +17704,7 @@
         <v>229</v>
       </c>
       <c r="J554" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="555" spans="1:10" x14ac:dyDescent="0.2">
@@ -17736,7 +17736,7 @@
         <v>227</v>
       </c>
       <c r="J555" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="556" spans="1:10" x14ac:dyDescent="0.2">
@@ -17823,7 +17823,7 @@
         <v>228</v>
       </c>
       <c r="J558" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="559" spans="1:10" x14ac:dyDescent="0.2">
@@ -17846,7 +17846,7 @@
         <v>227</v>
       </c>
       <c r="J559" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="560" spans="1:10" x14ac:dyDescent="0.2">
@@ -17878,7 +17878,7 @@
         <v>229</v>
       </c>
       <c r="J560" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="561" spans="1:10" x14ac:dyDescent="0.2">
@@ -17965,7 +17965,7 @@
         <v>228</v>
       </c>
       <c r="J563" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="564" spans="1:10" x14ac:dyDescent="0.2">
@@ -17988,7 +17988,7 @@
         <v>229</v>
       </c>
       <c r="J564" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="565" spans="1:10" x14ac:dyDescent="0.2">
@@ -18084,7 +18084,7 @@
         <v>223</v>
       </c>
       <c r="J567" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="568" spans="1:10" x14ac:dyDescent="0.2">
@@ -18240,7 +18240,7 @@
         <v>227</v>
       </c>
       <c r="J573" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="574" spans="1:10" x14ac:dyDescent="0.2">
@@ -18295,7 +18295,7 @@
         <v>227</v>
       </c>
       <c r="J575" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="576" spans="1:10" x14ac:dyDescent="0.2">
@@ -18318,7 +18318,7 @@
         <v>229</v>
       </c>
       <c r="J576" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="577" spans="1:10" x14ac:dyDescent="0.2">
@@ -18634,7 +18634,7 @@
         <v>227</v>
       </c>
       <c r="J587" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="588" spans="1:10" x14ac:dyDescent="0.2">
@@ -18666,7 +18666,7 @@
         <v>232</v>
       </c>
       <c r="J588" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="589" spans="1:10" x14ac:dyDescent="0.2">
@@ -18698,7 +18698,7 @@
         <v>232</v>
       </c>
       <c r="J589" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="590" spans="1:10" x14ac:dyDescent="0.2">
@@ -18730,7 +18730,7 @@
         <v>227</v>
       </c>
       <c r="J590" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="591" spans="1:10" x14ac:dyDescent="0.2">
@@ -18756,7 +18756,7 @@
         <v>223</v>
       </c>
       <c r="J591" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="592" spans="1:10" x14ac:dyDescent="0.2">
@@ -18788,7 +18788,7 @@
         <v>223</v>
       </c>
       <c r="J592" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="593" spans="1:10" x14ac:dyDescent="0.2">
@@ -18820,7 +18820,7 @@
         <v>223</v>
       </c>
       <c r="J593" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="594" spans="1:10" x14ac:dyDescent="0.2">
@@ -18852,7 +18852,7 @@
         <v>223</v>
       </c>
       <c r="J594" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="595" spans="1:10" x14ac:dyDescent="0.2">
@@ -18884,7 +18884,7 @@
         <v>223</v>
       </c>
       <c r="J595" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="596" spans="1:10" x14ac:dyDescent="0.2">
@@ -18910,7 +18910,7 @@
         <v>223</v>
       </c>
       <c r="J596" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="597" spans="1:10" x14ac:dyDescent="0.2">
@@ -18936,7 +18936,7 @@
         <v>223</v>
       </c>
       <c r="J597" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="598" spans="1:10" x14ac:dyDescent="0.2">
@@ -18962,7 +18962,7 @@
         <v>223</v>
       </c>
       <c r="J598" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="599" spans="1:10" x14ac:dyDescent="0.2">
@@ -19058,7 +19058,7 @@
         <v>225</v>
       </c>
       <c r="J601" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="602" spans="1:10" x14ac:dyDescent="0.2">
@@ -19081,7 +19081,7 @@
         <v>225</v>
       </c>
       <c r="J602" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="603" spans="1:10" x14ac:dyDescent="0.2">
@@ -19104,7 +19104,7 @@
         <v>228</v>
       </c>
       <c r="J603" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="604" spans="1:10" x14ac:dyDescent="0.2">
@@ -19200,7 +19200,7 @@
         <v>225</v>
       </c>
       <c r="J606" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="607" spans="1:10" x14ac:dyDescent="0.2">
@@ -19223,7 +19223,7 @@
         <v>228</v>
       </c>
       <c r="J607" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="608" spans="1:10" x14ac:dyDescent="0.2">
@@ -19246,7 +19246,7 @@
         <v>225</v>
       </c>
       <c r="J608" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="609" spans="1:10" x14ac:dyDescent="0.2">
@@ -19420,7 +19420,7 @@
         <v>226</v>
       </c>
       <c r="J614" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="615" spans="1:10" x14ac:dyDescent="0.2">
@@ -19484,7 +19484,7 @@
         <v>228</v>
       </c>
       <c r="J616" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="617" spans="1:10" x14ac:dyDescent="0.2">
@@ -19507,7 +19507,7 @@
         <v>225</v>
       </c>
       <c r="J617" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="618" spans="1:10" x14ac:dyDescent="0.2">
@@ -19530,7 +19530,7 @@
         <v>225</v>
       </c>
       <c r="J618" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="619" spans="1:10" x14ac:dyDescent="0.2">
@@ -19777,7 +19777,7 @@
         <v>225</v>
       </c>
       <c r="J626" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="627" spans="1:10" x14ac:dyDescent="0.2">
@@ -19800,7 +19800,7 @@
         <v>225</v>
       </c>
       <c r="J627" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="628" spans="1:10" x14ac:dyDescent="0.2">
@@ -19823,7 +19823,7 @@
         <v>228</v>
       </c>
       <c r="J628" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="629" spans="1:10" x14ac:dyDescent="0.2">
@@ -19855,7 +19855,7 @@
         <v>225</v>
       </c>
       <c r="J629" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="630" spans="1:10" x14ac:dyDescent="0.2">
@@ -19942,7 +19942,7 @@
         <v>228</v>
       </c>
       <c r="J632" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="633" spans="1:10" x14ac:dyDescent="0.2">
@@ -19965,7 +19965,7 @@
         <v>225</v>
       </c>
       <c r="J633" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="634" spans="1:10" x14ac:dyDescent="0.2">
@@ -20148,7 +20148,7 @@
         <v>227</v>
       </c>
       <c r="J639" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.2">
@@ -20180,7 +20180,7 @@
         <v>223</v>
       </c>
       <c r="J640" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.2">
@@ -20212,7 +20212,7 @@
         <v>232</v>
       </c>
       <c r="J641" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.2">
@@ -20244,7 +20244,7 @@
         <v>227</v>
       </c>
       <c r="J642" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="643" spans="1:10" x14ac:dyDescent="0.2">
@@ -20270,7 +20270,7 @@
         <v>232</v>
       </c>
       <c r="J643" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="644" spans="1:10" x14ac:dyDescent="0.2">
@@ -20476,7 +20476,7 @@
         <v>229</v>
       </c>
       <c r="J650" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="651" spans="1:10" x14ac:dyDescent="0.2">
@@ -20609,7 +20609,7 @@
         <v>228</v>
       </c>
       <c r="J655" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="656" spans="1:10" x14ac:dyDescent="0.2">
@@ -20673,7 +20673,7 @@
         <v>228</v>
       </c>
       <c r="J657" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="658" spans="1:11" x14ac:dyDescent="0.2">
@@ -20731,7 +20731,7 @@
         <v>229</v>
       </c>
       <c r="J659" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="660" spans="1:11" x14ac:dyDescent="0.2">
@@ -20829,7 +20829,7 @@
         <v>227</v>
       </c>
       <c r="J662" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K662" s="3"/>
     </row>
@@ -20853,7 +20853,7 @@
         <v>227</v>
       </c>
       <c r="J663" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K663" s="3"/>
     </row>
@@ -20877,7 +20877,7 @@
         <v>224</v>
       </c>
       <c r="J664" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K664" s="3"/>
     </row>
@@ -20943,7 +20943,7 @@
         <v>228</v>
       </c>
       <c r="J666" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K666" s="3"/>
     </row>
@@ -21000,7 +21000,7 @@
         <v>228</v>
       </c>
       <c r="J668" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K668" s="3"/>
     </row>
@@ -21024,7 +21024,7 @@
         <v>231</v>
       </c>
       <c r="J669" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K669" s="3"/>
     </row>
@@ -21361,7 +21361,7 @@
         <v>232</v>
       </c>
       <c r="J680" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="681" spans="1:10" x14ac:dyDescent="0.2">
@@ -21457,7 +21457,7 @@
         <v>232</v>
       </c>
       <c r="J683" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="684" spans="1:10" x14ac:dyDescent="0.2">
@@ -22126,7 +22126,7 @@
         <v>225</v>
       </c>
       <c r="J707" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="708" spans="1:10" x14ac:dyDescent="0.2">
@@ -22213,7 +22213,7 @@
         <v>225</v>
       </c>
       <c r="J710" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.2">
@@ -22236,7 +22236,7 @@
         <v>228</v>
       </c>
       <c r="J711" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.2">
@@ -22552,7 +22552,7 @@
         <v>225</v>
       </c>
       <c r="J722" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.2">
@@ -22639,7 +22639,7 @@
         <v>228</v>
       </c>
       <c r="J725" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="726" spans="1:10" x14ac:dyDescent="0.2">
@@ -22662,7 +22662,7 @@
         <v>225</v>
       </c>
       <c r="J726" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="727" spans="1:10" x14ac:dyDescent="0.2">
@@ -22758,7 +22758,7 @@
         <v>227</v>
       </c>
       <c r="J729" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="730" spans="1:10" x14ac:dyDescent="0.2">
@@ -22781,7 +22781,7 @@
         <v>228</v>
       </c>
       <c r="J730" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="731" spans="1:10" x14ac:dyDescent="0.2">
@@ -22804,7 +22804,7 @@
         <v>227</v>
       </c>
       <c r="J731" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>